<commit_message>
File handling write operation of excel
</commit_message>
<xml_diff>
--- a/Swital/Python_FileHandling/Read_Excel.xlsx
+++ b/Swital/Python_FileHandling/Read_Excel.xlsx
@@ -541,14 +541,145 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="C1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Data1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Data1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Data2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Data2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Data3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Data3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Data4</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Data4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Data5</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Data5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>User1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Pass1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>User2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Pass2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>User3</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Pass3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>User4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Pass4</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>User5</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Pass5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -559,14 +690,75 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>User1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Pass1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>User2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pass2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>User3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pass3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>User4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pass4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>User5</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pass5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>